<commit_message>
Reference added to Care Plan activity backbone element
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-careplan.xlsx
+++ b/output/StructureDefinition-careplan.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2345" uniqueCount="454">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2381" uniqueCount="458">
   <si>
     <t>Property</t>
   </si>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-07-17T16:21:50+02:00</t>
+    <t>2023-07-17T17:08:31+02:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -942,6 +942,19 @@
   </si>
   <si>
     <t>Attention Point on the observation</t>
+  </si>
+  <si>
+    <t>CarePlan.activity.extension:outcomeReference</t>
+  </si>
+  <si>
+    <t>outcomeReference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extension {http://example.org/fhir/fish/StructureDefinition/outcome-reference}
+</t>
+  </si>
+  <si>
+    <t>Outcome Reference</t>
   </si>
   <si>
     <t>CarePlan.activity.modifierExtension</t>
@@ -1729,7 +1742,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AN64"/>
+  <dimension ref="A1:AN65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -1738,9 +1751,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="40.75390625" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="42.03125" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="40.75390625" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="15.28125" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="3" max="3" width="17.5390625" customWidth="true" bestFit="true" hidden="true"/>
     <col min="4" max="4" width="38.4609375" customWidth="true" bestFit="true" hidden="true"/>
     <col min="6" max="6" width="2.203125" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="2.203125" customWidth="true" bestFit="true"/>
@@ -5560,7 +5573,7 @@
         <v>34</v>
       </c>
       <c r="G34" t="s" s="2">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="H34" t="s" s="2">
         <v>36</v>
@@ -5999,43 +6012,41 @@
         <v>295</v>
       </c>
       <c r="B38" t="s" s="2">
-        <v>295</v>
-      </c>
-      <c r="C38" s="2"/>
+        <v>288</v>
+      </c>
+      <c r="C38" t="s" s="2">
+        <v>296</v>
+      </c>
       <c r="D38" t="s" s="2">
-        <v>296</v>
+        <v>36</v>
       </c>
       <c r="E38" s="2"/>
       <c r="F38" t="s" s="2">
         <v>34</v>
       </c>
       <c r="G38" t="s" s="2">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="H38" t="s" s="2">
         <v>36</v>
       </c>
       <c r="I38" t="s" s="2">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="J38" t="s" s="2">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>88</v>
+        <v>297</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="M38" t="s" s="2">
-        <v>298</v>
-      </c>
-      <c r="N38" t="s" s="2">
-        <v>115</v>
-      </c>
-      <c r="O38" t="s" s="2">
-        <v>116</v>
-      </c>
+        <v>294</v>
+      </c>
+      <c r="N38" s="2"/>
+      <c r="O38" s="2"/>
       <c r="P38" t="s" s="2">
         <v>36</v>
       </c>
@@ -6083,7 +6094,7 @@
         <v>36</v>
       </c>
       <c r="AF38" t="s" s="2">
-        <v>299</v>
+        <v>289</v>
       </c>
       <c r="AG38" t="s" s="2">
         <v>34</v>
@@ -6092,7 +6103,7 @@
         <v>35</v>
       </c>
       <c r="AI38" t="s" s="2">
-        <v>36</v>
+        <v>100</v>
       </c>
       <c r="AJ38" t="s" s="2">
         <v>94</v>
@@ -6101,7 +6112,7 @@
         <v>36</v>
       </c>
       <c r="AL38" t="s" s="2">
-        <v>86</v>
+        <v>36</v>
       </c>
       <c r="AM38" t="s" s="2">
         <v>36</v>
@@ -6112,14 +6123,14 @@
     </row>
     <row r="39">
       <c r="A39" t="s" s="2">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B39" t="s" s="2">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" t="s" s="2">
-        <v>36</v>
+        <v>300</v>
       </c>
       <c r="E39" s="2"/>
       <c r="F39" t="s" s="2">
@@ -6132,13 +6143,13 @@
         <v>36</v>
       </c>
       <c r="I39" t="s" s="2">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="J39" t="s" s="2">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>177</v>
+        <v>88</v>
       </c>
       <c r="L39" t="s" s="2">
         <v>301</v>
@@ -6147,9 +6158,11 @@
         <v>302</v>
       </c>
       <c r="N39" t="s" s="2">
-        <v>303</v>
-      </c>
-      <c r="O39" s="2"/>
+        <v>115</v>
+      </c>
+      <c r="O39" t="s" s="2">
+        <v>116</v>
+      </c>
       <c r="P39" t="s" s="2">
         <v>36</v>
       </c>
@@ -6173,13 +6186,13 @@
         <v>36</v>
       </c>
       <c r="X39" t="s" s="2">
-        <v>182</v>
+        <v>36</v>
       </c>
       <c r="Y39" t="s" s="2">
-        <v>304</v>
+        <v>36</v>
       </c>
       <c r="Z39" t="s" s="2">
-        <v>305</v>
+        <v>36</v>
       </c>
       <c r="AA39" t="s" s="2">
         <v>36</v>
@@ -6197,7 +6210,7 @@
         <v>36</v>
       </c>
       <c r="AF39" t="s" s="2">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="AG39" t="s" s="2">
         <v>34</v>
@@ -6209,13 +6222,13 @@
         <v>36</v>
       </c>
       <c r="AJ39" t="s" s="2">
-        <v>55</v>
+        <v>94</v>
       </c>
       <c r="AK39" t="s" s="2">
         <v>36</v>
       </c>
       <c r="AL39" t="s" s="2">
-        <v>36</v>
+        <v>86</v>
       </c>
       <c r="AM39" t="s" s="2">
         <v>36</v>
@@ -6226,10 +6239,10 @@
     </row>
     <row r="40">
       <c r="A40" t="s" s="2">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B40" t="s" s="2">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" t="s" s="2">
@@ -6252,20 +6265,18 @@
         <v>36</v>
       </c>
       <c r="K40" t="s" s="2">
-        <v>261</v>
+        <v>177</v>
       </c>
       <c r="L40" t="s" s="2">
+        <v>305</v>
+      </c>
+      <c r="M40" t="s" s="2">
+        <v>306</v>
+      </c>
+      <c r="N40" t="s" s="2">
         <v>307</v>
       </c>
-      <c r="M40" t="s" s="2">
-        <v>308</v>
-      </c>
-      <c r="N40" t="s" s="2">
-        <v>309</v>
-      </c>
-      <c r="O40" t="s" s="2">
-        <v>310</v>
-      </c>
+      <c r="O40" s="2"/>
       <c r="P40" t="s" s="2">
         <v>36</v>
       </c>
@@ -6289,13 +6300,13 @@
         <v>36</v>
       </c>
       <c r="X40" t="s" s="2">
-        <v>36</v>
+        <v>182</v>
       </c>
       <c r="Y40" t="s" s="2">
-        <v>36</v>
+        <v>308</v>
       </c>
       <c r="Z40" t="s" s="2">
-        <v>36</v>
+        <v>309</v>
       </c>
       <c r="AA40" t="s" s="2">
         <v>36</v>
@@ -6313,7 +6324,7 @@
         <v>36</v>
       </c>
       <c r="AF40" t="s" s="2">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="AG40" t="s" s="2">
         <v>34</v>
@@ -6328,10 +6339,10 @@
         <v>55</v>
       </c>
       <c r="AK40" t="s" s="2">
-        <v>311</v>
+        <v>36</v>
       </c>
       <c r="AL40" t="s" s="2">
-        <v>312</v>
+        <v>36</v>
       </c>
       <c r="AM40" t="s" s="2">
         <v>36</v>
@@ -6342,10 +6353,10 @@
     </row>
     <row r="41">
       <c r="A41" t="s" s="2">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="B41" t="s" s="2">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" t="s" s="2">
@@ -6368,19 +6379,19 @@
         <v>36</v>
       </c>
       <c r="K41" t="s" s="2">
+        <v>261</v>
+      </c>
+      <c r="L41" t="s" s="2">
+        <v>311</v>
+      </c>
+      <c r="M41" t="s" s="2">
+        <v>312</v>
+      </c>
+      <c r="N41" t="s" s="2">
+        <v>313</v>
+      </c>
+      <c r="O41" t="s" s="2">
         <v>314</v>
-      </c>
-      <c r="L41" t="s" s="2">
-        <v>315</v>
-      </c>
-      <c r="M41" t="s" s="2">
-        <v>316</v>
-      </c>
-      <c r="N41" t="s" s="2">
-        <v>317</v>
-      </c>
-      <c r="O41" t="s" s="2">
-        <v>318</v>
       </c>
       <c r="P41" t="s" s="2">
         <v>36</v>
@@ -6429,7 +6440,7 @@
         <v>36</v>
       </c>
       <c r="AF41" t="s" s="2">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="AG41" t="s" s="2">
         <v>34</v>
@@ -6444,24 +6455,24 @@
         <v>55</v>
       </c>
       <c r="AK41" t="s" s="2">
-        <v>36</v>
+        <v>315</v>
       </c>
       <c r="AL41" t="s" s="2">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="AM41" t="s" s="2">
         <v>36</v>
       </c>
       <c r="AN41" t="s" s="2">
-        <v>320</v>
+        <v>36</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s" s="2">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="B42" t="s" s="2">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" t="s" s="2">
@@ -6472,7 +6483,7 @@
         <v>34</v>
       </c>
       <c r="G42" t="s" s="2">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="H42" t="s" s="2">
         <v>36</v>
@@ -6484,19 +6495,19 @@
         <v>36</v>
       </c>
       <c r="K42" t="s" s="2">
+        <v>318</v>
+      </c>
+      <c r="L42" t="s" s="2">
+        <v>319</v>
+      </c>
+      <c r="M42" t="s" s="2">
+        <v>320</v>
+      </c>
+      <c r="N42" t="s" s="2">
+        <v>321</v>
+      </c>
+      <c r="O42" t="s" s="2">
         <v>322</v>
-      </c>
-      <c r="L42" t="s" s="2">
-        <v>323</v>
-      </c>
-      <c r="M42" t="s" s="2">
-        <v>324</v>
-      </c>
-      <c r="N42" t="s" s="2">
-        <v>325</v>
-      </c>
-      <c r="O42" t="s" s="2">
-        <v>326</v>
       </c>
       <c r="P42" t="s" s="2">
         <v>36</v>
@@ -6545,39 +6556,39 @@
         <v>36</v>
       </c>
       <c r="AF42" t="s" s="2">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="AG42" t="s" s="2">
         <v>34</v>
       </c>
       <c r="AH42" t="s" s="2">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="AI42" t="s" s="2">
-        <v>327</v>
+        <v>36</v>
       </c>
       <c r="AJ42" t="s" s="2">
         <v>55</v>
       </c>
       <c r="AK42" t="s" s="2">
-        <v>328</v>
+        <v>36</v>
       </c>
       <c r="AL42" t="s" s="2">
-        <v>282</v>
+        <v>323</v>
       </c>
       <c r="AM42" t="s" s="2">
         <v>36</v>
       </c>
       <c r="AN42" t="s" s="2">
-        <v>36</v>
+        <v>324</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s" s="2">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="B43" t="s" s="2">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" t="s" s="2">
@@ -6600,17 +6611,19 @@
         <v>36</v>
       </c>
       <c r="K43" t="s" s="2">
-        <v>276</v>
+        <v>326</v>
       </c>
       <c r="L43" t="s" s="2">
+        <v>327</v>
+      </c>
+      <c r="M43" t="s" s="2">
+        <v>328</v>
+      </c>
+      <c r="N43" t="s" s="2">
+        <v>329</v>
+      </c>
+      <c r="O43" t="s" s="2">
         <v>330</v>
-      </c>
-      <c r="M43" t="s" s="2">
-        <v>331</v>
-      </c>
-      <c r="N43" s="2"/>
-      <c r="O43" t="s" s="2">
-        <v>332</v>
       </c>
       <c r="P43" t="s" s="2">
         <v>36</v>
@@ -6659,7 +6672,7 @@
         <v>36</v>
       </c>
       <c r="AF43" t="s" s="2">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="AG43" t="s" s="2">
         <v>34</v>
@@ -6668,16 +6681,16 @@
         <v>43</v>
       </c>
       <c r="AI43" t="s" s="2">
-        <v>327</v>
+        <v>331</v>
       </c>
       <c r="AJ43" t="s" s="2">
         <v>55</v>
       </c>
       <c r="AK43" t="s" s="2">
-        <v>36</v>
+        <v>332</v>
       </c>
       <c r="AL43" t="s" s="2">
-        <v>333</v>
+        <v>282</v>
       </c>
       <c r="AM43" t="s" s="2">
         <v>36</v>
@@ -6688,10 +6701,10 @@
     </row>
     <row r="44">
       <c r="A44" t="s" s="2">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B44" t="s" s="2">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" t="s" s="2">
@@ -6714,16 +6727,18 @@
         <v>36</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>187</v>
+        <v>276</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>284</v>
+        <v>334</v>
       </c>
       <c r="M44" t="s" s="2">
-        <v>285</v>
+        <v>335</v>
       </c>
       <c r="N44" s="2"/>
-      <c r="O44" s="2"/>
+      <c r="O44" t="s" s="2">
+        <v>336</v>
+      </c>
       <c r="P44" t="s" s="2">
         <v>36</v>
       </c>
@@ -6771,7 +6786,7 @@
         <v>36</v>
       </c>
       <c r="AF44" t="s" s="2">
-        <v>286</v>
+        <v>333</v>
       </c>
       <c r="AG44" t="s" s="2">
         <v>34</v>
@@ -6780,16 +6795,16 @@
         <v>43</v>
       </c>
       <c r="AI44" t="s" s="2">
-        <v>36</v>
+        <v>331</v>
       </c>
       <c r="AJ44" t="s" s="2">
-        <v>36</v>
+        <v>55</v>
       </c>
       <c r="AK44" t="s" s="2">
         <v>36</v>
       </c>
       <c r="AL44" t="s" s="2">
-        <v>287</v>
+        <v>337</v>
       </c>
       <c r="AM44" t="s" s="2">
         <v>36</v>
@@ -6800,21 +6815,21 @@
     </row>
     <row r="45">
       <c r="A45" t="s" s="2">
-        <v>335</v>
+        <v>338</v>
       </c>
       <c r="B45" t="s" s="2">
-        <v>335</v>
+        <v>338</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" t="s" s="2">
-        <v>112</v>
+        <v>36</v>
       </c>
       <c r="E45" s="2"/>
       <c r="F45" t="s" s="2">
         <v>34</v>
       </c>
       <c r="G45" t="s" s="2">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="H45" t="s" s="2">
         <v>36</v>
@@ -6826,17 +6841,15 @@
         <v>36</v>
       </c>
       <c r="K45" t="s" s="2">
-        <v>88</v>
+        <v>187</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>336</v>
+        <v>284</v>
       </c>
       <c r="M45" t="s" s="2">
-        <v>337</v>
-      </c>
-      <c r="N45" t="s" s="2">
-        <v>115</v>
-      </c>
+        <v>285</v>
+      </c>
+      <c r="N45" s="2"/>
       <c r="O45" s="2"/>
       <c r="P45" t="s" s="2">
         <v>36</v>
@@ -6885,19 +6898,19 @@
         <v>36</v>
       </c>
       <c r="AF45" t="s" s="2">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="AG45" t="s" s="2">
         <v>34</v>
       </c>
       <c r="AH45" t="s" s="2">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="AI45" t="s" s="2">
         <v>36</v>
       </c>
       <c r="AJ45" t="s" s="2">
-        <v>94</v>
+        <v>36</v>
       </c>
       <c r="AK45" t="s" s="2">
         <v>36</v>
@@ -6914,14 +6927,14 @@
     </row>
     <row r="46">
       <c r="A46" t="s" s="2">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="B46" t="s" s="2">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" t="s" s="2">
-        <v>296</v>
+        <v>112</v>
       </c>
       <c r="E46" s="2"/>
       <c r="F46" t="s" s="2">
@@ -6934,26 +6947,24 @@
         <v>36</v>
       </c>
       <c r="I46" t="s" s="2">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="J46" t="s" s="2">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="K46" t="s" s="2">
         <v>88</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>297</v>
+        <v>340</v>
       </c>
       <c r="M46" t="s" s="2">
-        <v>298</v>
+        <v>341</v>
       </c>
       <c r="N46" t="s" s="2">
         <v>115</v>
       </c>
-      <c r="O46" t="s" s="2">
-        <v>116</v>
-      </c>
+      <c r="O46" s="2"/>
       <c r="P46" t="s" s="2">
         <v>36</v>
       </c>
@@ -7001,7 +7012,7 @@
         <v>36</v>
       </c>
       <c r="AF46" t="s" s="2">
-        <v>299</v>
+        <v>289</v>
       </c>
       <c r="AG46" t="s" s="2">
         <v>34</v>
@@ -7019,7 +7030,7 @@
         <v>36</v>
       </c>
       <c r="AL46" t="s" s="2">
-        <v>86</v>
+        <v>287</v>
       </c>
       <c r="AM46" t="s" s="2">
         <v>36</v>
@@ -7030,43 +7041,45 @@
     </row>
     <row r="47">
       <c r="A47" t="s" s="2">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="B47" t="s" s="2">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" t="s" s="2">
-        <v>36</v>
+        <v>300</v>
       </c>
       <c r="E47" s="2"/>
       <c r="F47" t="s" s="2">
         <v>34</v>
       </c>
       <c r="G47" t="s" s="2">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="H47" t="s" s="2">
         <v>36</v>
       </c>
       <c r="I47" t="s" s="2">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="J47" t="s" s="2">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="K47" t="s" s="2">
-        <v>63</v>
+        <v>88</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>340</v>
+        <v>301</v>
       </c>
       <c r="M47" t="s" s="2">
-        <v>341</v>
-      </c>
-      <c r="N47" s="2"/>
+        <v>302</v>
+      </c>
+      <c r="N47" t="s" s="2">
+        <v>115</v>
+      </c>
       <c r="O47" t="s" s="2">
-        <v>342</v>
+        <v>116</v>
       </c>
       <c r="P47" t="s" s="2">
         <v>36</v>
@@ -7091,13 +7104,13 @@
         <v>36</v>
       </c>
       <c r="X47" t="s" s="2">
-        <v>162</v>
+        <v>36</v>
       </c>
       <c r="Y47" t="s" s="2">
-        <v>343</v>
+        <v>36</v>
       </c>
       <c r="Z47" t="s" s="2">
-        <v>344</v>
+        <v>36</v>
       </c>
       <c r="AA47" t="s" s="2">
         <v>36</v>
@@ -7115,25 +7128,25 @@
         <v>36</v>
       </c>
       <c r="AF47" t="s" s="2">
-        <v>339</v>
+        <v>303</v>
       </c>
       <c r="AG47" t="s" s="2">
         <v>34</v>
       </c>
       <c r="AH47" t="s" s="2">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="AI47" t="s" s="2">
         <v>36</v>
       </c>
       <c r="AJ47" t="s" s="2">
-        <v>55</v>
+        <v>94</v>
       </c>
       <c r="AK47" t="s" s="2">
         <v>36</v>
       </c>
       <c r="AL47" t="s" s="2">
-        <v>345</v>
+        <v>86</v>
       </c>
       <c r="AM47" t="s" s="2">
         <v>36</v>
@@ -7144,10 +7157,10 @@
     </row>
     <row r="48">
       <c r="A48" t="s" s="2">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="B48" t="s" s="2">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" t="s" s="2">
@@ -7158,7 +7171,7 @@
         <v>34</v>
       </c>
       <c r="G48" t="s" s="2">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="H48" t="s" s="2">
         <v>36</v>
@@ -7170,17 +7183,17 @@
         <v>36</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>347</v>
+        <v>63</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>130</v>
+        <v>344</v>
       </c>
       <c r="M48" t="s" s="2">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="N48" s="2"/>
       <c r="O48" t="s" s="2">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="P48" t="s" s="2">
         <v>36</v>
@@ -7205,13 +7218,13 @@
         <v>36</v>
       </c>
       <c r="X48" t="s" s="2">
-        <v>36</v>
+        <v>162</v>
       </c>
       <c r="Y48" t="s" s="2">
-        <v>36</v>
+        <v>347</v>
       </c>
       <c r="Z48" t="s" s="2">
-        <v>36</v>
+        <v>348</v>
       </c>
       <c r="AA48" t="s" s="2">
         <v>36</v>
@@ -7229,13 +7242,13 @@
         <v>36</v>
       </c>
       <c r="AF48" t="s" s="2">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="AG48" t="s" s="2">
         <v>34</v>
       </c>
       <c r="AH48" t="s" s="2">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="AI48" t="s" s="2">
         <v>36</v>
@@ -7244,10 +7257,10 @@
         <v>55</v>
       </c>
       <c r="AK48" t="s" s="2">
-        <v>132</v>
+        <v>36</v>
       </c>
       <c r="AL48" t="s" s="2">
-        <v>133</v>
+        <v>349</v>
       </c>
       <c r="AM48" t="s" s="2">
         <v>36</v>
@@ -7284,19 +7297,17 @@
         <v>36</v>
       </c>
       <c r="K49" t="s" s="2">
-        <v>57</v>
+        <v>351</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="M49" t="s" s="2">
-        <v>351</v>
-      </c>
-      <c r="N49" t="s" s="2">
-        <v>137</v>
-      </c>
+        <v>352</v>
+      </c>
+      <c r="N49" s="2"/>
       <c r="O49" t="s" s="2">
-        <v>349</v>
+        <v>353</v>
       </c>
       <c r="P49" t="s" s="2">
         <v>36</v>
@@ -7360,7 +7371,7 @@
         <v>55</v>
       </c>
       <c r="AK49" t="s" s="2">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="AL49" t="s" s="2">
         <v>133</v>
@@ -7374,10 +7385,10 @@
     </row>
     <row r="50">
       <c r="A50" t="s" s="2">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="B50" t="s" s="2">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="C50" s="2"/>
       <c r="D50" t="s" s="2">
@@ -7388,7 +7399,7 @@
         <v>34</v>
       </c>
       <c r="G50" t="s" s="2">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="H50" t="s" s="2">
         <v>36</v>
@@ -7400,19 +7411,19 @@
         <v>36</v>
       </c>
       <c r="K50" t="s" s="2">
-        <v>177</v>
+        <v>57</v>
       </c>
       <c r="L50" t="s" s="2">
+        <v>135</v>
+      </c>
+      <c r="M50" t="s" s="2">
+        <v>355</v>
+      </c>
+      <c r="N50" t="s" s="2">
+        <v>137</v>
+      </c>
+      <c r="O50" t="s" s="2">
         <v>353</v>
-      </c>
-      <c r="M50" t="s" s="2">
-        <v>354</v>
-      </c>
-      <c r="N50" t="s" s="2">
-        <v>355</v>
-      </c>
-      <c r="O50" t="s" s="2">
-        <v>356</v>
       </c>
       <c r="P50" t="s" s="2">
         <v>36</v>
@@ -7437,13 +7448,13 @@
         <v>36</v>
       </c>
       <c r="X50" t="s" s="2">
-        <v>182</v>
+        <v>36</v>
       </c>
       <c r="Y50" t="s" s="2">
-        <v>357</v>
+        <v>36</v>
       </c>
       <c r="Z50" t="s" s="2">
-        <v>358</v>
+        <v>36</v>
       </c>
       <c r="AA50" t="s" s="2">
         <v>36</v>
@@ -7461,13 +7472,13 @@
         <v>36</v>
       </c>
       <c r="AF50" t="s" s="2">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="AG50" t="s" s="2">
         <v>34</v>
       </c>
       <c r="AH50" t="s" s="2">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="AI50" t="s" s="2">
         <v>36</v>
@@ -7476,24 +7487,24 @@
         <v>55</v>
       </c>
       <c r="AK50" t="s" s="2">
-        <v>359</v>
+        <v>138</v>
       </c>
       <c r="AL50" t="s" s="2">
-        <v>360</v>
+        <v>133</v>
       </c>
       <c r="AM50" t="s" s="2">
         <v>36</v>
       </c>
       <c r="AN50" t="s" s="2">
-        <v>361</v>
+        <v>36</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s" s="2">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="B51" t="s" s="2">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" t="s" s="2">
@@ -7504,7 +7515,7 @@
         <v>34</v>
       </c>
       <c r="G51" t="s" s="2">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="H51" t="s" s="2">
         <v>36</v>
@@ -7519,15 +7530,17 @@
         <v>177</v>
       </c>
       <c r="L51" t="s" s="2">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="M51" t="s" s="2">
-        <v>364</v>
+        <v>358</v>
       </c>
       <c r="N51" t="s" s="2">
-        <v>365</v>
-      </c>
-      <c r="O51" s="2"/>
+        <v>359</v>
+      </c>
+      <c r="O51" t="s" s="2">
+        <v>360</v>
+      </c>
       <c r="P51" t="s" s="2">
         <v>36</v>
       </c>
@@ -7554,10 +7567,10 @@
         <v>182</v>
       </c>
       <c r="Y51" t="s" s="2">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="Z51" t="s" s="2">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="AA51" t="s" s="2">
         <v>36</v>
@@ -7575,13 +7588,13 @@
         <v>36</v>
       </c>
       <c r="AF51" t="s" s="2">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="AG51" t="s" s="2">
         <v>34</v>
       </c>
       <c r="AH51" t="s" s="2">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="AI51" t="s" s="2">
         <v>36</v>
@@ -7590,24 +7603,24 @@
         <v>55</v>
       </c>
       <c r="AK51" t="s" s="2">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="AL51" t="s" s="2">
-        <v>36</v>
+        <v>364</v>
       </c>
       <c r="AM51" t="s" s="2">
         <v>36</v>
       </c>
       <c r="AN51" t="s" s="2">
-        <v>36</v>
+        <v>365</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s" s="2">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="B52" t="s" s="2">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" t="s" s="2">
@@ -7630,16 +7643,16 @@
         <v>36</v>
       </c>
       <c r="K52" t="s" s="2">
-        <v>370</v>
+        <v>177</v>
       </c>
       <c r="L52" t="s" s="2">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="M52" t="s" s="2">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="N52" t="s" s="2">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="O52" s="2"/>
       <c r="P52" t="s" s="2">
@@ -7665,13 +7678,13 @@
         <v>36</v>
       </c>
       <c r="X52" t="s" s="2">
-        <v>36</v>
+        <v>182</v>
       </c>
       <c r="Y52" t="s" s="2">
-        <v>36</v>
+        <v>370</v>
       </c>
       <c r="Z52" t="s" s="2">
-        <v>36</v>
+        <v>371</v>
       </c>
       <c r="AA52" t="s" s="2">
         <v>36</v>
@@ -7689,7 +7702,7 @@
         <v>36</v>
       </c>
       <c r="AF52" t="s" s="2">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="AG52" t="s" s="2">
         <v>34</v>
@@ -7704,7 +7717,7 @@
         <v>55</v>
       </c>
       <c r="AK52" t="s" s="2">
-        <v>256</v>
+        <v>372</v>
       </c>
       <c r="AL52" t="s" s="2">
         <v>36</v>
@@ -7718,10 +7731,10 @@
     </row>
     <row r="53">
       <c r="A53" t="s" s="2">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B53" t="s" s="2">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C53" s="2"/>
       <c r="D53" t="s" s="2">
@@ -7744,7 +7757,7 @@
         <v>36</v>
       </c>
       <c r="K53" t="s" s="2">
-        <v>268</v>
+        <v>374</v>
       </c>
       <c r="L53" t="s" s="2">
         <v>375</v>
@@ -7752,10 +7765,10 @@
       <c r="M53" t="s" s="2">
         <v>376</v>
       </c>
-      <c r="N53" s="2"/>
-      <c r="O53" t="s" s="2">
+      <c r="N53" t="s" s="2">
         <v>377</v>
       </c>
+      <c r="O53" s="2"/>
       <c r="P53" t="s" s="2">
         <v>36</v>
       </c>
@@ -7803,7 +7816,7 @@
         <v>36</v>
       </c>
       <c r="AF53" t="s" s="2">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="AG53" t="s" s="2">
         <v>34</v>
@@ -7818,10 +7831,10 @@
         <v>55</v>
       </c>
       <c r="AK53" t="s" s="2">
-        <v>36</v>
+        <v>256</v>
       </c>
       <c r="AL53" t="s" s="2">
-        <v>273</v>
+        <v>36</v>
       </c>
       <c r="AM53" t="s" s="2">
         <v>36</v>
@@ -7843,22 +7856,22 @@
       </c>
       <c r="E54" s="2"/>
       <c r="F54" t="s" s="2">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="G54" t="s" s="2">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="H54" t="s" s="2">
         <v>36</v>
       </c>
       <c r="I54" t="s" s="2">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="J54" t="s" s="2">
         <v>36</v>
       </c>
       <c r="K54" t="s" s="2">
-        <v>63</v>
+        <v>268</v>
       </c>
       <c r="L54" t="s" s="2">
         <v>379</v>
@@ -7866,11 +7879,9 @@
       <c r="M54" t="s" s="2">
         <v>380</v>
       </c>
-      <c r="N54" t="s" s="2">
+      <c r="N54" s="2"/>
+      <c r="O54" t="s" s="2">
         <v>381</v>
-      </c>
-      <c r="O54" t="s" s="2">
-        <v>382</v>
       </c>
       <c r="P54" t="s" s="2">
         <v>36</v>
@@ -7895,13 +7906,13 @@
         <v>36</v>
       </c>
       <c r="X54" t="s" s="2">
-        <v>162</v>
+        <v>36</v>
       </c>
       <c r="Y54" t="s" s="2">
-        <v>383</v>
+        <v>36</v>
       </c>
       <c r="Z54" t="s" s="2">
-        <v>384</v>
+        <v>36</v>
       </c>
       <c r="AA54" t="s" s="2">
         <v>36</v>
@@ -7922,10 +7933,10 @@
         <v>378</v>
       </c>
       <c r="AG54" t="s" s="2">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="AH54" t="s" s="2">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="AI54" t="s" s="2">
         <v>36</v>
@@ -7934,24 +7945,24 @@
         <v>55</v>
       </c>
       <c r="AK54" t="s" s="2">
-        <v>385</v>
+        <v>36</v>
       </c>
       <c r="AL54" t="s" s="2">
-        <v>386</v>
+        <v>273</v>
       </c>
       <c r="AM54" t="s" s="2">
         <v>36</v>
       </c>
       <c r="AN54" t="s" s="2">
-        <v>387</v>
+        <v>36</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s" s="2">
-        <v>388</v>
+        <v>382</v>
       </c>
       <c r="B55" t="s" s="2">
-        <v>388</v>
+        <v>382</v>
       </c>
       <c r="C55" s="2"/>
       <c r="D55" t="s" s="2">
@@ -7959,7 +7970,7 @@
       </c>
       <c r="E55" s="2"/>
       <c r="F55" t="s" s="2">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="G55" t="s" s="2">
         <v>43</v>
@@ -7968,24 +7979,26 @@
         <v>36</v>
       </c>
       <c r="I55" t="s" s="2">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="J55" t="s" s="2">
         <v>36</v>
       </c>
       <c r="K55" t="s" s="2">
-        <v>177</v>
+        <v>63</v>
       </c>
       <c r="L55" t="s" s="2">
-        <v>389</v>
+        <v>383</v>
       </c>
       <c r="M55" t="s" s="2">
-        <v>390</v>
+        <v>384</v>
       </c>
       <c r="N55" t="s" s="2">
-        <v>391</v>
-      </c>
-      <c r="O55" s="2"/>
+        <v>385</v>
+      </c>
+      <c r="O55" t="s" s="2">
+        <v>386</v>
+      </c>
       <c r="P55" t="s" s="2">
         <v>36</v>
       </c>
@@ -8009,13 +8022,13 @@
         <v>36</v>
       </c>
       <c r="X55" t="s" s="2">
-        <v>36</v>
+        <v>162</v>
       </c>
       <c r="Y55" t="s" s="2">
-        <v>36</v>
+        <v>387</v>
       </c>
       <c r="Z55" t="s" s="2">
-        <v>36</v>
+        <v>388</v>
       </c>
       <c r="AA55" t="s" s="2">
         <v>36</v>
@@ -8033,10 +8046,10 @@
         <v>36</v>
       </c>
       <c r="AF55" t="s" s="2">
-        <v>388</v>
+        <v>382</v>
       </c>
       <c r="AG55" t="s" s="2">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="AH55" t="s" s="2">
         <v>43</v>
@@ -8048,24 +8061,24 @@
         <v>55</v>
       </c>
       <c r="AK55" t="s" s="2">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="AL55" t="s" s="2">
-        <v>36</v>
+        <v>390</v>
       </c>
       <c r="AM55" t="s" s="2">
         <v>36</v>
       </c>
       <c r="AN55" t="s" s="2">
-        <v>36</v>
+        <v>391</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s" s="2">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B56" t="s" s="2">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C56" s="2"/>
       <c r="D56" t="s" s="2">
@@ -8082,32 +8095,28 @@
         <v>36</v>
       </c>
       <c r="I56" t="s" s="2">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="J56" t="s" s="2">
         <v>36</v>
       </c>
       <c r="K56" t="s" s="2">
+        <v>177</v>
+      </c>
+      <c r="L56" t="s" s="2">
+        <v>393</v>
+      </c>
+      <c r="M56" t="s" s="2">
         <v>394</v>
       </c>
-      <c r="L56" t="s" s="2">
+      <c r="N56" t="s" s="2">
         <v>395</v>
       </c>
-      <c r="M56" t="s" s="2">
-        <v>396</v>
-      </c>
-      <c r="N56" t="s" s="2">
-        <v>397</v>
-      </c>
-      <c r="O56" t="s" s="2">
-        <v>398</v>
-      </c>
+      <c r="O56" s="2"/>
       <c r="P56" t="s" s="2">
         <v>36</v>
       </c>
-      <c r="Q56" t="s" s="2">
-        <v>399</v>
-      </c>
+      <c r="Q56" s="2"/>
       <c r="R56" t="s" s="2">
         <v>36</v>
       </c>
@@ -8151,7 +8160,7 @@
         <v>36</v>
       </c>
       <c r="AF56" t="s" s="2">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="AG56" t="s" s="2">
         <v>34</v>
@@ -8166,10 +8175,10 @@
         <v>55</v>
       </c>
       <c r="AK56" t="s" s="2">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="AL56" t="s" s="2">
-        <v>401</v>
+        <v>36</v>
       </c>
       <c r="AM56" t="s" s="2">
         <v>36</v>
@@ -8180,10 +8189,10 @@
     </row>
     <row r="57">
       <c r="A57" t="s" s="2">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="B57" t="s" s="2">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="C57" s="2"/>
       <c r="D57" t="s" s="2">
@@ -8200,28 +8209,32 @@
         <v>36</v>
       </c>
       <c r="I57" t="s" s="2">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="J57" t="s" s="2">
         <v>36</v>
       </c>
       <c r="K57" t="s" s="2">
+        <v>398</v>
+      </c>
+      <c r="L57" t="s" s="2">
+        <v>399</v>
+      </c>
+      <c r="M57" t="s" s="2">
+        <v>400</v>
+      </c>
+      <c r="N57" t="s" s="2">
+        <v>401</v>
+      </c>
+      <c r="O57" t="s" s="2">
+        <v>402</v>
+      </c>
+      <c r="P57" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="Q57" t="s" s="2">
         <v>403</v>
       </c>
-      <c r="L57" t="s" s="2">
-        <v>404</v>
-      </c>
-      <c r="M57" t="s" s="2">
-        <v>405</v>
-      </c>
-      <c r="N57" s="2"/>
-      <c r="O57" t="s" s="2">
-        <v>406</v>
-      </c>
-      <c r="P57" t="s" s="2">
-        <v>36</v>
-      </c>
-      <c r="Q57" s="2"/>
       <c r="R57" t="s" s="2">
         <v>36</v>
       </c>
@@ -8265,7 +8278,7 @@
         <v>36</v>
       </c>
       <c r="AF57" t="s" s="2">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="AG57" t="s" s="2">
         <v>34</v>
@@ -8280,24 +8293,24 @@
         <v>55</v>
       </c>
       <c r="AK57" t="s" s="2">
-        <v>220</v>
+        <v>404</v>
       </c>
       <c r="AL57" t="s" s="2">
-        <v>221</v>
+        <v>405</v>
       </c>
       <c r="AM57" t="s" s="2">
         <v>36</v>
       </c>
       <c r="AN57" t="s" s="2">
-        <v>407</v>
+        <v>36</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s" s="2">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="B58" t="s" s="2">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="C58" s="2"/>
       <c r="D58" t="s" s="2">
@@ -8320,19 +8333,17 @@
         <v>36</v>
       </c>
       <c r="K58" t="s" s="2">
+        <v>407</v>
+      </c>
+      <c r="L58" t="s" s="2">
+        <v>408</v>
+      </c>
+      <c r="M58" t="s" s="2">
         <v>409</v>
       </c>
-      <c r="L58" t="s" s="2">
+      <c r="N58" s="2"/>
+      <c r="O58" t="s" s="2">
         <v>410</v>
-      </c>
-      <c r="M58" t="s" s="2">
-        <v>411</v>
-      </c>
-      <c r="N58" t="s" s="2">
-        <v>412</v>
-      </c>
-      <c r="O58" t="s" s="2">
-        <v>413</v>
       </c>
       <c r="P58" t="s" s="2">
         <v>36</v>
@@ -8381,7 +8392,7 @@
         <v>36</v>
       </c>
       <c r="AF58" t="s" s="2">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="AG58" t="s" s="2">
         <v>34</v>
@@ -8396,24 +8407,24 @@
         <v>55</v>
       </c>
       <c r="AK58" t="s" s="2">
-        <v>36</v>
+        <v>220</v>
       </c>
       <c r="AL58" t="s" s="2">
-        <v>414</v>
+        <v>221</v>
       </c>
       <c r="AM58" t="s" s="2">
         <v>36</v>
       </c>
       <c r="AN58" t="s" s="2">
-        <v>415</v>
+        <v>411</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s" s="2">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="B59" t="s" s="2">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="C59" s="2"/>
       <c r="D59" t="s" s="2">
@@ -8424,7 +8435,7 @@
         <v>34</v>
       </c>
       <c r="G59" t="s" s="2">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="H59" t="s" s="2">
         <v>36</v>
@@ -8436,19 +8447,19 @@
         <v>36</v>
       </c>
       <c r="K59" t="s" s="2">
+        <v>413</v>
+      </c>
+      <c r="L59" t="s" s="2">
+        <v>414</v>
+      </c>
+      <c r="M59" t="s" s="2">
+        <v>415</v>
+      </c>
+      <c r="N59" t="s" s="2">
+        <v>416</v>
+      </c>
+      <c r="O59" t="s" s="2">
         <v>417</v>
-      </c>
-      <c r="L59" t="s" s="2">
-        <v>418</v>
-      </c>
-      <c r="M59" t="s" s="2">
-        <v>419</v>
-      </c>
-      <c r="N59" t="s" s="2">
-        <v>420</v>
-      </c>
-      <c r="O59" t="s" s="2">
-        <v>413</v>
       </c>
       <c r="P59" t="s" s="2">
         <v>36</v>
@@ -8497,13 +8508,13 @@
         <v>36</v>
       </c>
       <c r="AF59" t="s" s="2">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="AG59" t="s" s="2">
         <v>34</v>
       </c>
       <c r="AH59" t="s" s="2">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="AI59" t="s" s="2">
         <v>36</v>
@@ -8512,24 +8523,24 @@
         <v>55</v>
       </c>
       <c r="AK59" t="s" s="2">
-        <v>421</v>
+        <v>36</v>
       </c>
       <c r="AL59" t="s" s="2">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="AM59" t="s" s="2">
         <v>36</v>
       </c>
       <c r="AN59" t="s" s="2">
-        <v>423</v>
+        <v>419</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s" s="2">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="B60" t="s" s="2">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="C60" s="2"/>
       <c r="D60" t="s" s="2">
@@ -8540,7 +8551,7 @@
         <v>34</v>
       </c>
       <c r="G60" t="s" s="2">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="H60" t="s" s="2">
         <v>36</v>
@@ -8552,16 +8563,20 @@
         <v>36</v>
       </c>
       <c r="K60" t="s" s="2">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="L60" t="s" s="2">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="M60" t="s" s="2">
-        <v>427</v>
-      </c>
-      <c r="N60" s="2"/>
-      <c r="O60" s="2"/>
+        <v>423</v>
+      </c>
+      <c r="N60" t="s" s="2">
+        <v>424</v>
+      </c>
+      <c r="O60" t="s" s="2">
+        <v>417</v>
+      </c>
       <c r="P60" t="s" s="2">
         <v>36</v>
       </c>
@@ -8585,13 +8600,13 @@
         <v>36</v>
       </c>
       <c r="X60" t="s" s="2">
-        <v>182</v>
+        <v>36</v>
       </c>
       <c r="Y60" t="s" s="2">
-        <v>428</v>
+        <v>36</v>
       </c>
       <c r="Z60" t="s" s="2">
-        <v>429</v>
+        <v>36</v>
       </c>
       <c r="AA60" t="s" s="2">
         <v>36</v>
@@ -8609,13 +8624,13 @@
         <v>36</v>
       </c>
       <c r="AF60" t="s" s="2">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="AG60" t="s" s="2">
         <v>34</v>
       </c>
       <c r="AH60" t="s" s="2">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="AI60" t="s" s="2">
         <v>36</v>
@@ -8624,28 +8639,28 @@
         <v>55</v>
       </c>
       <c r="AK60" t="s" s="2">
-        <v>36</v>
+        <v>425</v>
       </c>
       <c r="AL60" t="s" s="2">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="AM60" t="s" s="2">
         <v>36</v>
       </c>
       <c r="AN60" t="s" s="2">
-        <v>431</v>
+        <v>427</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s" s="2">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="B61" t="s" s="2">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="C61" s="2"/>
       <c r="D61" t="s" s="2">
-        <v>433</v>
+        <v>36</v>
       </c>
       <c r="E61" s="2"/>
       <c r="F61" t="s" s="2">
@@ -8664,18 +8679,16 @@
         <v>36</v>
       </c>
       <c r="K61" t="s" s="2">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="L61" t="s" s="2">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="M61" t="s" s="2">
-        <v>436</v>
+        <v>431</v>
       </c>
       <c r="N61" s="2"/>
-      <c r="O61" t="s" s="2">
-        <v>437</v>
-      </c>
+      <c r="O61" s="2"/>
       <c r="P61" t="s" s="2">
         <v>36</v>
       </c>
@@ -8699,13 +8712,13 @@
         <v>36</v>
       </c>
       <c r="X61" t="s" s="2">
-        <v>36</v>
+        <v>182</v>
       </c>
       <c r="Y61" t="s" s="2">
-        <v>36</v>
+        <v>432</v>
       </c>
       <c r="Z61" t="s" s="2">
-        <v>36</v>
+        <v>433</v>
       </c>
       <c r="AA61" t="s" s="2">
         <v>36</v>
@@ -8723,7 +8736,7 @@
         <v>36</v>
       </c>
       <c r="AF61" t="s" s="2">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="AG61" t="s" s="2">
         <v>34</v>
@@ -8741,25 +8754,25 @@
         <v>36</v>
       </c>
       <c r="AL61" t="s" s="2">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="AM61" t="s" s="2">
         <v>36</v>
       </c>
       <c r="AN61" t="s" s="2">
-        <v>439</v>
+        <v>435</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s" s="2">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="B62" t="s" s="2">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="C62" s="2"/>
       <c r="D62" t="s" s="2">
-        <v>36</v>
+        <v>437</v>
       </c>
       <c r="E62" s="2"/>
       <c r="F62" t="s" s="2">
@@ -8778,16 +8791,18 @@
         <v>36</v>
       </c>
       <c r="K62" t="s" s="2">
-        <v>434</v>
+        <v>438</v>
       </c>
       <c r="L62" t="s" s="2">
+        <v>439</v>
+      </c>
+      <c r="M62" t="s" s="2">
+        <v>440</v>
+      </c>
+      <c r="N62" s="2"/>
+      <c r="O62" t="s" s="2">
         <v>441</v>
       </c>
-      <c r="M62" t="s" s="2">
-        <v>442</v>
-      </c>
-      <c r="N62" s="2"/>
-      <c r="O62" s="2"/>
       <c r="P62" t="s" s="2">
         <v>36</v>
       </c>
@@ -8835,7 +8850,7 @@
         <v>36</v>
       </c>
       <c r="AF62" t="s" s="2">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="AG62" t="s" s="2">
         <v>34</v>
@@ -8853,21 +8868,21 @@
         <v>36</v>
       </c>
       <c r="AL62" t="s" s="2">
+        <v>442</v>
+      </c>
+      <c r="AM62" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="AN62" t="s" s="2">
         <v>443</v>
-      </c>
-      <c r="AM62" t="s" s="2">
-        <v>36</v>
-      </c>
-      <c r="AN62" t="s" s="2">
-        <v>444</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s" s="2">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B63" t="s" s="2">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C63" s="2"/>
       <c r="D63" t="s" s="2">
@@ -8890,13 +8905,13 @@
         <v>36</v>
       </c>
       <c r="K63" t="s" s="2">
-        <v>187</v>
+        <v>438</v>
       </c>
       <c r="L63" t="s" s="2">
+        <v>445</v>
+      </c>
+      <c r="M63" t="s" s="2">
         <v>446</v>
-      </c>
-      <c r="M63" t="s" s="2">
-        <v>447</v>
       </c>
       <c r="N63" s="2"/>
       <c r="O63" s="2"/>
@@ -8947,7 +8962,7 @@
         <v>36</v>
       </c>
       <c r="AF63" t="s" s="2">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="AG63" t="s" s="2">
         <v>34</v>
@@ -8965,13 +8980,13 @@
         <v>36</v>
       </c>
       <c r="AL63" t="s" s="2">
+        <v>447</v>
+      </c>
+      <c r="AM63" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="AN63" t="s" s="2">
         <v>448</v>
-      </c>
-      <c r="AM63" t="s" s="2">
-        <v>36</v>
-      </c>
-      <c r="AN63" t="s" s="2">
-        <v>320</v>
       </c>
     </row>
     <row r="64">
@@ -8990,7 +9005,7 @@
         <v>34</v>
       </c>
       <c r="G64" t="s" s="2">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="H64" t="s" s="2">
         <v>36</v>
@@ -9002,7 +9017,7 @@
         <v>36</v>
       </c>
       <c r="K64" t="s" s="2">
-        <v>314</v>
+        <v>187</v>
       </c>
       <c r="L64" t="s" s="2">
         <v>450</v>
@@ -9011,9 +9026,7 @@
         <v>451</v>
       </c>
       <c r="N64" s="2"/>
-      <c r="O64" t="s" s="2">
-        <v>452</v>
-      </c>
+      <c r="O64" s="2"/>
       <c r="P64" t="s" s="2">
         <v>36</v>
       </c>
@@ -9067,7 +9080,7 @@
         <v>34</v>
       </c>
       <c r="AH64" t="s" s="2">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="AI64" t="s" s="2">
         <v>36</v>
@@ -9076,16 +9089,130 @@
         <v>55</v>
       </c>
       <c r="AK64" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="AL64" t="s" s="2">
+        <v>452</v>
+      </c>
+      <c r="AM64" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="AN64" t="s" s="2">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="s" s="2">
         <v>453</v>
       </c>
-      <c r="AL64" t="s" s="2">
-        <v>319</v>
-      </c>
-      <c r="AM64" t="s" s="2">
-        <v>36</v>
-      </c>
-      <c r="AN64" t="s" s="2">
-        <v>320</v>
+      <c r="B65" t="s" s="2">
+        <v>453</v>
+      </c>
+      <c r="C65" s="2"/>
+      <c r="D65" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="E65" s="2"/>
+      <c r="F65" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="G65" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="H65" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="I65" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="J65" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="K65" t="s" s="2">
+        <v>318</v>
+      </c>
+      <c r="L65" t="s" s="2">
+        <v>454</v>
+      </c>
+      <c r="M65" t="s" s="2">
+        <v>455</v>
+      </c>
+      <c r="N65" s="2"/>
+      <c r="O65" t="s" s="2">
+        <v>456</v>
+      </c>
+      <c r="P65" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="Q65" s="2"/>
+      <c r="R65" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="S65" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="T65" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="U65" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="V65" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="W65" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="X65" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="Y65" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="Z65" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="AA65" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="AB65" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="AC65" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="AD65" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="AE65" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="AF65" t="s" s="2">
+        <v>453</v>
+      </c>
+      <c r="AG65" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="AH65" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AI65" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="AJ65" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="AK65" t="s" s="2">
+        <v>457</v>
+      </c>
+      <c r="AL65" t="s" s="2">
+        <v>323</v>
+      </c>
+      <c r="AM65" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="AN65" t="s" s="2">
+        <v>324</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Latest updates on the Care Plan model
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-careplan.xlsx
+++ b/output/StructureDefinition-careplan.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2381" uniqueCount="458">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2417" uniqueCount="462">
   <si>
     <t>Property</t>
   </si>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-07-17T17:08:31+02:00</t>
+    <t>2023-07-17T17:22:35+02:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -955,6 +955,19 @@
   </si>
   <si>
     <t>Outcome Reference</t>
+  </si>
+  <si>
+    <t>CarePlan.activity.extension:Reference</t>
+  </si>
+  <si>
+    <t>Reference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extension {http://example.org/fhir/fish/StructureDefinition/reference}
+</t>
+  </si>
+  <si>
+    <t>Type of observation made by the contributor</t>
   </si>
   <si>
     <t>CarePlan.activity.modifierExtension</t>
@@ -1742,7 +1755,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AN65"/>
+  <dimension ref="A1:AN66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -5796,7 +5809,7 @@
       </c>
       <c r="E36" s="2"/>
       <c r="F36" t="s" s="2">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="G36" t="s" s="2">
         <v>35</v>
@@ -6126,43 +6139,41 @@
         <v>299</v>
       </c>
       <c r="B39" t="s" s="2">
-        <v>299</v>
-      </c>
-      <c r="C39" s="2"/>
+        <v>288</v>
+      </c>
+      <c r="C39" t="s" s="2">
+        <v>300</v>
+      </c>
       <c r="D39" t="s" s="2">
-        <v>300</v>
+        <v>36</v>
       </c>
       <c r="E39" s="2"/>
       <c r="F39" t="s" s="2">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="G39" t="s" s="2">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="H39" t="s" s="2">
         <v>36</v>
       </c>
       <c r="I39" t="s" s="2">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="J39" t="s" s="2">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>88</v>
+        <v>301</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="M39" t="s" s="2">
         <v>302</v>
       </c>
-      <c r="N39" t="s" s="2">
-        <v>115</v>
-      </c>
-      <c r="O39" t="s" s="2">
-        <v>116</v>
-      </c>
+      <c r="N39" s="2"/>
+      <c r="O39" s="2"/>
       <c r="P39" t="s" s="2">
         <v>36</v>
       </c>
@@ -6210,7 +6221,7 @@
         <v>36</v>
       </c>
       <c r="AF39" t="s" s="2">
-        <v>303</v>
+        <v>289</v>
       </c>
       <c r="AG39" t="s" s="2">
         <v>34</v>
@@ -6219,7 +6230,7 @@
         <v>35</v>
       </c>
       <c r="AI39" t="s" s="2">
-        <v>36</v>
+        <v>100</v>
       </c>
       <c r="AJ39" t="s" s="2">
         <v>94</v>
@@ -6228,7 +6239,7 @@
         <v>36</v>
       </c>
       <c r="AL39" t="s" s="2">
-        <v>86</v>
+        <v>36</v>
       </c>
       <c r="AM39" t="s" s="2">
         <v>36</v>
@@ -6239,14 +6250,14 @@
     </row>
     <row r="40">
       <c r="A40" t="s" s="2">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B40" t="s" s="2">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" t="s" s="2">
-        <v>36</v>
+        <v>304</v>
       </c>
       <c r="E40" s="2"/>
       <c r="F40" t="s" s="2">
@@ -6259,13 +6270,13 @@
         <v>36</v>
       </c>
       <c r="I40" t="s" s="2">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="J40" t="s" s="2">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="K40" t="s" s="2">
-        <v>177</v>
+        <v>88</v>
       </c>
       <c r="L40" t="s" s="2">
         <v>305</v>
@@ -6274,9 +6285,11 @@
         <v>306</v>
       </c>
       <c r="N40" t="s" s="2">
-        <v>307</v>
-      </c>
-      <c r="O40" s="2"/>
+        <v>115</v>
+      </c>
+      <c r="O40" t="s" s="2">
+        <v>116</v>
+      </c>
       <c r="P40" t="s" s="2">
         <v>36</v>
       </c>
@@ -6300,13 +6313,13 @@
         <v>36</v>
       </c>
       <c r="X40" t="s" s="2">
-        <v>182</v>
+        <v>36</v>
       </c>
       <c r="Y40" t="s" s="2">
-        <v>308</v>
+        <v>36</v>
       </c>
       <c r="Z40" t="s" s="2">
-        <v>309</v>
+        <v>36</v>
       </c>
       <c r="AA40" t="s" s="2">
         <v>36</v>
@@ -6324,7 +6337,7 @@
         <v>36</v>
       </c>
       <c r="AF40" t="s" s="2">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="AG40" t="s" s="2">
         <v>34</v>
@@ -6336,13 +6349,13 @@
         <v>36</v>
       </c>
       <c r="AJ40" t="s" s="2">
-        <v>55</v>
+        <v>94</v>
       </c>
       <c r="AK40" t="s" s="2">
         <v>36</v>
       </c>
       <c r="AL40" t="s" s="2">
-        <v>36</v>
+        <v>86</v>
       </c>
       <c r="AM40" t="s" s="2">
         <v>36</v>
@@ -6353,10 +6366,10 @@
     </row>
     <row r="41">
       <c r="A41" t="s" s="2">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B41" t="s" s="2">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" t="s" s="2">
@@ -6379,20 +6392,18 @@
         <v>36</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>261</v>
+        <v>177</v>
       </c>
       <c r="L41" t="s" s="2">
+        <v>309</v>
+      </c>
+      <c r="M41" t="s" s="2">
+        <v>310</v>
+      </c>
+      <c r="N41" t="s" s="2">
         <v>311</v>
       </c>
-      <c r="M41" t="s" s="2">
-        <v>312</v>
-      </c>
-      <c r="N41" t="s" s="2">
-        <v>313</v>
-      </c>
-      <c r="O41" t="s" s="2">
-        <v>314</v>
-      </c>
+      <c r="O41" s="2"/>
       <c r="P41" t="s" s="2">
         <v>36</v>
       </c>
@@ -6416,13 +6427,13 @@
         <v>36</v>
       </c>
       <c r="X41" t="s" s="2">
-        <v>36</v>
+        <v>182</v>
       </c>
       <c r="Y41" t="s" s="2">
-        <v>36</v>
+        <v>312</v>
       </c>
       <c r="Z41" t="s" s="2">
-        <v>36</v>
+        <v>313</v>
       </c>
       <c r="AA41" t="s" s="2">
         <v>36</v>
@@ -6440,7 +6451,7 @@
         <v>36</v>
       </c>
       <c r="AF41" t="s" s="2">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="AG41" t="s" s="2">
         <v>34</v>
@@ -6455,10 +6466,10 @@
         <v>55</v>
       </c>
       <c r="AK41" t="s" s="2">
-        <v>315</v>
+        <v>36</v>
       </c>
       <c r="AL41" t="s" s="2">
-        <v>316</v>
+        <v>36</v>
       </c>
       <c r="AM41" t="s" s="2">
         <v>36</v>
@@ -6469,10 +6480,10 @@
     </row>
     <row r="42">
       <c r="A42" t="s" s="2">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="B42" t="s" s="2">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" t="s" s="2">
@@ -6495,19 +6506,19 @@
         <v>36</v>
       </c>
       <c r="K42" t="s" s="2">
+        <v>261</v>
+      </c>
+      <c r="L42" t="s" s="2">
+        <v>315</v>
+      </c>
+      <c r="M42" t="s" s="2">
+        <v>316</v>
+      </c>
+      <c r="N42" t="s" s="2">
+        <v>317</v>
+      </c>
+      <c r="O42" t="s" s="2">
         <v>318</v>
-      </c>
-      <c r="L42" t="s" s="2">
-        <v>319</v>
-      </c>
-      <c r="M42" t="s" s="2">
-        <v>320</v>
-      </c>
-      <c r="N42" t="s" s="2">
-        <v>321</v>
-      </c>
-      <c r="O42" t="s" s="2">
-        <v>322</v>
       </c>
       <c r="P42" t="s" s="2">
         <v>36</v>
@@ -6556,7 +6567,7 @@
         <v>36</v>
       </c>
       <c r="AF42" t="s" s="2">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="AG42" t="s" s="2">
         <v>34</v>
@@ -6571,24 +6582,24 @@
         <v>55</v>
       </c>
       <c r="AK42" t="s" s="2">
-        <v>36</v>
+        <v>319</v>
       </c>
       <c r="AL42" t="s" s="2">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="AM42" t="s" s="2">
         <v>36</v>
       </c>
       <c r="AN42" t="s" s="2">
-        <v>324</v>
+        <v>36</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s" s="2">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="B43" t="s" s="2">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" t="s" s="2">
@@ -6599,7 +6610,7 @@
         <v>34</v>
       </c>
       <c r="G43" t="s" s="2">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="H43" t="s" s="2">
         <v>36</v>
@@ -6611,19 +6622,19 @@
         <v>36</v>
       </c>
       <c r="K43" t="s" s="2">
+        <v>322</v>
+      </c>
+      <c r="L43" t="s" s="2">
+        <v>323</v>
+      </c>
+      <c r="M43" t="s" s="2">
+        <v>324</v>
+      </c>
+      <c r="N43" t="s" s="2">
+        <v>325</v>
+      </c>
+      <c r="O43" t="s" s="2">
         <v>326</v>
-      </c>
-      <c r="L43" t="s" s="2">
-        <v>327</v>
-      </c>
-      <c r="M43" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="N43" t="s" s="2">
-        <v>329</v>
-      </c>
-      <c r="O43" t="s" s="2">
-        <v>330</v>
       </c>
       <c r="P43" t="s" s="2">
         <v>36</v>
@@ -6672,39 +6683,39 @@
         <v>36</v>
       </c>
       <c r="AF43" t="s" s="2">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="AG43" t="s" s="2">
         <v>34</v>
       </c>
       <c r="AH43" t="s" s="2">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="AI43" t="s" s="2">
-        <v>331</v>
+        <v>36</v>
       </c>
       <c r="AJ43" t="s" s="2">
         <v>55</v>
       </c>
       <c r="AK43" t="s" s="2">
-        <v>332</v>
+        <v>36</v>
       </c>
       <c r="AL43" t="s" s="2">
-        <v>282</v>
+        <v>327</v>
       </c>
       <c r="AM43" t="s" s="2">
         <v>36</v>
       </c>
       <c r="AN43" t="s" s="2">
-        <v>36</v>
+        <v>328</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s" s="2">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="B44" t="s" s="2">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" t="s" s="2">
@@ -6727,17 +6738,19 @@
         <v>36</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>276</v>
+        <v>330</v>
       </c>
       <c r="L44" t="s" s="2">
+        <v>331</v>
+      </c>
+      <c r="M44" t="s" s="2">
+        <v>332</v>
+      </c>
+      <c r="N44" t="s" s="2">
+        <v>333</v>
+      </c>
+      <c r="O44" t="s" s="2">
         <v>334</v>
-      </c>
-      <c r="M44" t="s" s="2">
-        <v>335</v>
-      </c>
-      <c r="N44" s="2"/>
-      <c r="O44" t="s" s="2">
-        <v>336</v>
       </c>
       <c r="P44" t="s" s="2">
         <v>36</v>
@@ -6786,7 +6799,7 @@
         <v>36</v>
       </c>
       <c r="AF44" t="s" s="2">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="AG44" t="s" s="2">
         <v>34</v>
@@ -6795,16 +6808,16 @@
         <v>43</v>
       </c>
       <c r="AI44" t="s" s="2">
-        <v>331</v>
+        <v>335</v>
       </c>
       <c r="AJ44" t="s" s="2">
         <v>55</v>
       </c>
       <c r="AK44" t="s" s="2">
-        <v>36</v>
+        <v>336</v>
       </c>
       <c r="AL44" t="s" s="2">
-        <v>337</v>
+        <v>282</v>
       </c>
       <c r="AM44" t="s" s="2">
         <v>36</v>
@@ -6815,10 +6828,10 @@
     </row>
     <row r="45">
       <c r="A45" t="s" s="2">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B45" t="s" s="2">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" t="s" s="2">
@@ -6841,16 +6854,18 @@
         <v>36</v>
       </c>
       <c r="K45" t="s" s="2">
-        <v>187</v>
+        <v>276</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>284</v>
+        <v>338</v>
       </c>
       <c r="M45" t="s" s="2">
-        <v>285</v>
+        <v>339</v>
       </c>
       <c r="N45" s="2"/>
-      <c r="O45" s="2"/>
+      <c r="O45" t="s" s="2">
+        <v>340</v>
+      </c>
       <c r="P45" t="s" s="2">
         <v>36</v>
       </c>
@@ -6898,7 +6913,7 @@
         <v>36</v>
       </c>
       <c r="AF45" t="s" s="2">
-        <v>286</v>
+        <v>337</v>
       </c>
       <c r="AG45" t="s" s="2">
         <v>34</v>
@@ -6907,16 +6922,16 @@
         <v>43</v>
       </c>
       <c r="AI45" t="s" s="2">
-        <v>36</v>
+        <v>335</v>
       </c>
       <c r="AJ45" t="s" s="2">
-        <v>36</v>
+        <v>55</v>
       </c>
       <c r="AK45" t="s" s="2">
         <v>36</v>
       </c>
       <c r="AL45" t="s" s="2">
-        <v>287</v>
+        <v>341</v>
       </c>
       <c r="AM45" t="s" s="2">
         <v>36</v>
@@ -6927,21 +6942,21 @@
     </row>
     <row r="46">
       <c r="A46" t="s" s="2">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="B46" t="s" s="2">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" t="s" s="2">
-        <v>112</v>
+        <v>36</v>
       </c>
       <c r="E46" s="2"/>
       <c r="F46" t="s" s="2">
         <v>34</v>
       </c>
       <c r="G46" t="s" s="2">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="H46" t="s" s="2">
         <v>36</v>
@@ -6953,17 +6968,15 @@
         <v>36</v>
       </c>
       <c r="K46" t="s" s="2">
-        <v>88</v>
+        <v>187</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>340</v>
+        <v>284</v>
       </c>
       <c r="M46" t="s" s="2">
-        <v>341</v>
-      </c>
-      <c r="N46" t="s" s="2">
-        <v>115</v>
-      </c>
+        <v>285</v>
+      </c>
+      <c r="N46" s="2"/>
       <c r="O46" s="2"/>
       <c r="P46" t="s" s="2">
         <v>36</v>
@@ -7012,19 +7025,19 @@
         <v>36</v>
       </c>
       <c r="AF46" t="s" s="2">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="AG46" t="s" s="2">
         <v>34</v>
       </c>
       <c r="AH46" t="s" s="2">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="AI46" t="s" s="2">
         <v>36</v>
       </c>
       <c r="AJ46" t="s" s="2">
-        <v>94</v>
+        <v>36</v>
       </c>
       <c r="AK46" t="s" s="2">
         <v>36</v>
@@ -7041,14 +7054,14 @@
     </row>
     <row r="47">
       <c r="A47" t="s" s="2">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="B47" t="s" s="2">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" t="s" s="2">
-        <v>300</v>
+        <v>112</v>
       </c>
       <c r="E47" s="2"/>
       <c r="F47" t="s" s="2">
@@ -7061,26 +7074,24 @@
         <v>36</v>
       </c>
       <c r="I47" t="s" s="2">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="J47" t="s" s="2">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="K47" t="s" s="2">
         <v>88</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>301</v>
+        <v>344</v>
       </c>
       <c r="M47" t="s" s="2">
-        <v>302</v>
+        <v>345</v>
       </c>
       <c r="N47" t="s" s="2">
         <v>115</v>
       </c>
-      <c r="O47" t="s" s="2">
-        <v>116</v>
-      </c>
+      <c r="O47" s="2"/>
       <c r="P47" t="s" s="2">
         <v>36</v>
       </c>
@@ -7128,7 +7139,7 @@
         <v>36</v>
       </c>
       <c r="AF47" t="s" s="2">
-        <v>303</v>
+        <v>289</v>
       </c>
       <c r="AG47" t="s" s="2">
         <v>34</v>
@@ -7146,7 +7157,7 @@
         <v>36</v>
       </c>
       <c r="AL47" t="s" s="2">
-        <v>86</v>
+        <v>287</v>
       </c>
       <c r="AM47" t="s" s="2">
         <v>36</v>
@@ -7157,43 +7168,45 @@
     </row>
     <row r="48">
       <c r="A48" t="s" s="2">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="B48" t="s" s="2">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" t="s" s="2">
-        <v>36</v>
+        <v>304</v>
       </c>
       <c r="E48" s="2"/>
       <c r="F48" t="s" s="2">
         <v>34</v>
       </c>
       <c r="G48" t="s" s="2">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="H48" t="s" s="2">
         <v>36</v>
       </c>
       <c r="I48" t="s" s="2">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="J48" t="s" s="2">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>63</v>
+        <v>88</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>344</v>
+        <v>305</v>
       </c>
       <c r="M48" t="s" s="2">
-        <v>345</v>
-      </c>
-      <c r="N48" s="2"/>
+        <v>306</v>
+      </c>
+      <c r="N48" t="s" s="2">
+        <v>115</v>
+      </c>
       <c r="O48" t="s" s="2">
-        <v>346</v>
+        <v>116</v>
       </c>
       <c r="P48" t="s" s="2">
         <v>36</v>
@@ -7218,13 +7231,13 @@
         <v>36</v>
       </c>
       <c r="X48" t="s" s="2">
-        <v>162</v>
+        <v>36</v>
       </c>
       <c r="Y48" t="s" s="2">
-        <v>347</v>
+        <v>36</v>
       </c>
       <c r="Z48" t="s" s="2">
-        <v>348</v>
+        <v>36</v>
       </c>
       <c r="AA48" t="s" s="2">
         <v>36</v>
@@ -7242,25 +7255,25 @@
         <v>36</v>
       </c>
       <c r="AF48" t="s" s="2">
-        <v>343</v>
+        <v>307</v>
       </c>
       <c r="AG48" t="s" s="2">
         <v>34</v>
       </c>
       <c r="AH48" t="s" s="2">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="AI48" t="s" s="2">
         <v>36</v>
       </c>
       <c r="AJ48" t="s" s="2">
-        <v>55</v>
+        <v>94</v>
       </c>
       <c r="AK48" t="s" s="2">
         <v>36</v>
       </c>
       <c r="AL48" t="s" s="2">
-        <v>349</v>
+        <v>86</v>
       </c>
       <c r="AM48" t="s" s="2">
         <v>36</v>
@@ -7271,10 +7284,10 @@
     </row>
     <row r="49">
       <c r="A49" t="s" s="2">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="B49" t="s" s="2">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" t="s" s="2">
@@ -7285,7 +7298,7 @@
         <v>34</v>
       </c>
       <c r="G49" t="s" s="2">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="H49" t="s" s="2">
         <v>36</v>
@@ -7297,17 +7310,17 @@
         <v>36</v>
       </c>
       <c r="K49" t="s" s="2">
-        <v>351</v>
+        <v>63</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>130</v>
+        <v>348</v>
       </c>
       <c r="M49" t="s" s="2">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="N49" s="2"/>
       <c r="O49" t="s" s="2">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="P49" t="s" s="2">
         <v>36</v>
@@ -7332,13 +7345,13 @@
         <v>36</v>
       </c>
       <c r="X49" t="s" s="2">
-        <v>36</v>
+        <v>162</v>
       </c>
       <c r="Y49" t="s" s="2">
-        <v>36</v>
+        <v>351</v>
       </c>
       <c r="Z49" t="s" s="2">
-        <v>36</v>
+        <v>352</v>
       </c>
       <c r="AA49" t="s" s="2">
         <v>36</v>
@@ -7356,13 +7369,13 @@
         <v>36</v>
       </c>
       <c r="AF49" t="s" s="2">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="AG49" t="s" s="2">
         <v>34</v>
       </c>
       <c r="AH49" t="s" s="2">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="AI49" t="s" s="2">
         <v>36</v>
@@ -7371,10 +7384,10 @@
         <v>55</v>
       </c>
       <c r="AK49" t="s" s="2">
-        <v>132</v>
+        <v>36</v>
       </c>
       <c r="AL49" t="s" s="2">
-        <v>133</v>
+        <v>353</v>
       </c>
       <c r="AM49" t="s" s="2">
         <v>36</v>
@@ -7411,19 +7424,17 @@
         <v>36</v>
       </c>
       <c r="K50" t="s" s="2">
-        <v>57</v>
+        <v>355</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="M50" t="s" s="2">
-        <v>355</v>
-      </c>
-      <c r="N50" t="s" s="2">
-        <v>137</v>
-      </c>
+        <v>356</v>
+      </c>
+      <c r="N50" s="2"/>
       <c r="O50" t="s" s="2">
-        <v>353</v>
+        <v>357</v>
       </c>
       <c r="P50" t="s" s="2">
         <v>36</v>
@@ -7487,7 +7498,7 @@
         <v>55</v>
       </c>
       <c r="AK50" t="s" s="2">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="AL50" t="s" s="2">
         <v>133</v>
@@ -7501,10 +7512,10 @@
     </row>
     <row r="51">
       <c r="A51" t="s" s="2">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="B51" t="s" s="2">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" t="s" s="2">
@@ -7515,7 +7526,7 @@
         <v>34</v>
       </c>
       <c r="G51" t="s" s="2">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="H51" t="s" s="2">
         <v>36</v>
@@ -7527,19 +7538,19 @@
         <v>36</v>
       </c>
       <c r="K51" t="s" s="2">
-        <v>177</v>
+        <v>57</v>
       </c>
       <c r="L51" t="s" s="2">
+        <v>135</v>
+      </c>
+      <c r="M51" t="s" s="2">
+        <v>359</v>
+      </c>
+      <c r="N51" t="s" s="2">
+        <v>137</v>
+      </c>
+      <c r="O51" t="s" s="2">
         <v>357</v>
-      </c>
-      <c r="M51" t="s" s="2">
-        <v>358</v>
-      </c>
-      <c r="N51" t="s" s="2">
-        <v>359</v>
-      </c>
-      <c r="O51" t="s" s="2">
-        <v>360</v>
       </c>
       <c r="P51" t="s" s="2">
         <v>36</v>
@@ -7564,13 +7575,13 @@
         <v>36</v>
       </c>
       <c r="X51" t="s" s="2">
-        <v>182</v>
+        <v>36</v>
       </c>
       <c r="Y51" t="s" s="2">
-        <v>361</v>
+        <v>36</v>
       </c>
       <c r="Z51" t="s" s="2">
-        <v>362</v>
+        <v>36</v>
       </c>
       <c r="AA51" t="s" s="2">
         <v>36</v>
@@ -7588,13 +7599,13 @@
         <v>36</v>
       </c>
       <c r="AF51" t="s" s="2">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="AG51" t="s" s="2">
         <v>34</v>
       </c>
       <c r="AH51" t="s" s="2">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="AI51" t="s" s="2">
         <v>36</v>
@@ -7603,24 +7614,24 @@
         <v>55</v>
       </c>
       <c r="AK51" t="s" s="2">
-        <v>363</v>
+        <v>138</v>
       </c>
       <c r="AL51" t="s" s="2">
-        <v>364</v>
+        <v>133</v>
       </c>
       <c r="AM51" t="s" s="2">
         <v>36</v>
       </c>
       <c r="AN51" t="s" s="2">
-        <v>365</v>
+        <v>36</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s" s="2">
-        <v>366</v>
+        <v>360</v>
       </c>
       <c r="B52" t="s" s="2">
-        <v>366</v>
+        <v>360</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" t="s" s="2">
@@ -7631,7 +7642,7 @@
         <v>34</v>
       </c>
       <c r="G52" t="s" s="2">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="H52" t="s" s="2">
         <v>36</v>
@@ -7646,15 +7657,17 @@
         <v>177</v>
       </c>
       <c r="L52" t="s" s="2">
-        <v>367</v>
+        <v>361</v>
       </c>
       <c r="M52" t="s" s="2">
-        <v>368</v>
+        <v>362</v>
       </c>
       <c r="N52" t="s" s="2">
-        <v>369</v>
-      </c>
-      <c r="O52" s="2"/>
+        <v>363</v>
+      </c>
+      <c r="O52" t="s" s="2">
+        <v>364</v>
+      </c>
       <c r="P52" t="s" s="2">
         <v>36</v>
       </c>
@@ -7681,10 +7694,10 @@
         <v>182</v>
       </c>
       <c r="Y52" t="s" s="2">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="Z52" t="s" s="2">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="AA52" t="s" s="2">
         <v>36</v>
@@ -7702,13 +7715,13 @@
         <v>36</v>
       </c>
       <c r="AF52" t="s" s="2">
-        <v>366</v>
+        <v>360</v>
       </c>
       <c r="AG52" t="s" s="2">
         <v>34</v>
       </c>
       <c r="AH52" t="s" s="2">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="AI52" t="s" s="2">
         <v>36</v>
@@ -7717,24 +7730,24 @@
         <v>55</v>
       </c>
       <c r="AK52" t="s" s="2">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="AL52" t="s" s="2">
-        <v>36</v>
+        <v>368</v>
       </c>
       <c r="AM52" t="s" s="2">
         <v>36</v>
       </c>
       <c r="AN52" t="s" s="2">
-        <v>36</v>
+        <v>369</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s" s="2">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="B53" t="s" s="2">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="C53" s="2"/>
       <c r="D53" t="s" s="2">
@@ -7757,16 +7770,16 @@
         <v>36</v>
       </c>
       <c r="K53" t="s" s="2">
-        <v>374</v>
+        <v>177</v>
       </c>
       <c r="L53" t="s" s="2">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="M53" t="s" s="2">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="N53" t="s" s="2">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="O53" s="2"/>
       <c r="P53" t="s" s="2">
@@ -7792,13 +7805,13 @@
         <v>36</v>
       </c>
       <c r="X53" t="s" s="2">
-        <v>36</v>
+        <v>182</v>
       </c>
       <c r="Y53" t="s" s="2">
-        <v>36</v>
+        <v>374</v>
       </c>
       <c r="Z53" t="s" s="2">
-        <v>36</v>
+        <v>375</v>
       </c>
       <c r="AA53" t="s" s="2">
         <v>36</v>
@@ -7816,7 +7829,7 @@
         <v>36</v>
       </c>
       <c r="AF53" t="s" s="2">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="AG53" t="s" s="2">
         <v>34</v>
@@ -7831,7 +7844,7 @@
         <v>55</v>
       </c>
       <c r="AK53" t="s" s="2">
-        <v>256</v>
+        <v>376</v>
       </c>
       <c r="AL53" t="s" s="2">
         <v>36</v>
@@ -7845,10 +7858,10 @@
     </row>
     <row r="54">
       <c r="A54" t="s" s="2">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B54" t="s" s="2">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C54" s="2"/>
       <c r="D54" t="s" s="2">
@@ -7871,7 +7884,7 @@
         <v>36</v>
       </c>
       <c r="K54" t="s" s="2">
-        <v>268</v>
+        <v>378</v>
       </c>
       <c r="L54" t="s" s="2">
         <v>379</v>
@@ -7879,10 +7892,10 @@
       <c r="M54" t="s" s="2">
         <v>380</v>
       </c>
-      <c r="N54" s="2"/>
-      <c r="O54" t="s" s="2">
+      <c r="N54" t="s" s="2">
         <v>381</v>
       </c>
+      <c r="O54" s="2"/>
       <c r="P54" t="s" s="2">
         <v>36</v>
       </c>
@@ -7930,7 +7943,7 @@
         <v>36</v>
       </c>
       <c r="AF54" t="s" s="2">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="AG54" t="s" s="2">
         <v>34</v>
@@ -7945,10 +7958,10 @@
         <v>55</v>
       </c>
       <c r="AK54" t="s" s="2">
-        <v>36</v>
+        <v>256</v>
       </c>
       <c r="AL54" t="s" s="2">
-        <v>273</v>
+        <v>36</v>
       </c>
       <c r="AM54" t="s" s="2">
         <v>36</v>
@@ -7970,22 +7983,22 @@
       </c>
       <c r="E55" s="2"/>
       <c r="F55" t="s" s="2">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="G55" t="s" s="2">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="H55" t="s" s="2">
         <v>36</v>
       </c>
       <c r="I55" t="s" s="2">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="J55" t="s" s="2">
         <v>36</v>
       </c>
       <c r="K55" t="s" s="2">
-        <v>63</v>
+        <v>268</v>
       </c>
       <c r="L55" t="s" s="2">
         <v>383</v>
@@ -7993,11 +8006,9 @@
       <c r="M55" t="s" s="2">
         <v>384</v>
       </c>
-      <c r="N55" t="s" s="2">
+      <c r="N55" s="2"/>
+      <c r="O55" t="s" s="2">
         <v>385</v>
-      </c>
-      <c r="O55" t="s" s="2">
-        <v>386</v>
       </c>
       <c r="P55" t="s" s="2">
         <v>36</v>
@@ -8022,13 +8033,13 @@
         <v>36</v>
       </c>
       <c r="X55" t="s" s="2">
-        <v>162</v>
+        <v>36</v>
       </c>
       <c r="Y55" t="s" s="2">
-        <v>387</v>
+        <v>36</v>
       </c>
       <c r="Z55" t="s" s="2">
-        <v>388</v>
+        <v>36</v>
       </c>
       <c r="AA55" t="s" s="2">
         <v>36</v>
@@ -8049,10 +8060,10 @@
         <v>382</v>
       </c>
       <c r="AG55" t="s" s="2">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="AH55" t="s" s="2">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="AI55" t="s" s="2">
         <v>36</v>
@@ -8061,24 +8072,24 @@
         <v>55</v>
       </c>
       <c r="AK55" t="s" s="2">
-        <v>389</v>
+        <v>36</v>
       </c>
       <c r="AL55" t="s" s="2">
-        <v>390</v>
+        <v>273</v>
       </c>
       <c r="AM55" t="s" s="2">
         <v>36</v>
       </c>
       <c r="AN55" t="s" s="2">
-        <v>391</v>
+        <v>36</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s" s="2">
-        <v>392</v>
+        <v>386</v>
       </c>
       <c r="B56" t="s" s="2">
-        <v>392</v>
+        <v>386</v>
       </c>
       <c r="C56" s="2"/>
       <c r="D56" t="s" s="2">
@@ -8086,7 +8097,7 @@
       </c>
       <c r="E56" s="2"/>
       <c r="F56" t="s" s="2">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="G56" t="s" s="2">
         <v>43</v>
@@ -8095,24 +8106,26 @@
         <v>36</v>
       </c>
       <c r="I56" t="s" s="2">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="J56" t="s" s="2">
         <v>36</v>
       </c>
       <c r="K56" t="s" s="2">
-        <v>177</v>
+        <v>63</v>
       </c>
       <c r="L56" t="s" s="2">
-        <v>393</v>
+        <v>387</v>
       </c>
       <c r="M56" t="s" s="2">
-        <v>394</v>
+        <v>388</v>
       </c>
       <c r="N56" t="s" s="2">
-        <v>395</v>
-      </c>
-      <c r="O56" s="2"/>
+        <v>389</v>
+      </c>
+      <c r="O56" t="s" s="2">
+        <v>390</v>
+      </c>
       <c r="P56" t="s" s="2">
         <v>36</v>
       </c>
@@ -8136,13 +8149,13 @@
         <v>36</v>
       </c>
       <c r="X56" t="s" s="2">
-        <v>36</v>
+        <v>162</v>
       </c>
       <c r="Y56" t="s" s="2">
-        <v>36</v>
+        <v>391</v>
       </c>
       <c r="Z56" t="s" s="2">
-        <v>36</v>
+        <v>392</v>
       </c>
       <c r="AA56" t="s" s="2">
         <v>36</v>
@@ -8160,10 +8173,10 @@
         <v>36</v>
       </c>
       <c r="AF56" t="s" s="2">
-        <v>392</v>
+        <v>386</v>
       </c>
       <c r="AG56" t="s" s="2">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="AH56" t="s" s="2">
         <v>43</v>
@@ -8175,24 +8188,24 @@
         <v>55</v>
       </c>
       <c r="AK56" t="s" s="2">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="AL56" t="s" s="2">
-        <v>36</v>
+        <v>394</v>
       </c>
       <c r="AM56" t="s" s="2">
         <v>36</v>
       </c>
       <c r="AN56" t="s" s="2">
-        <v>36</v>
+        <v>395</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s" s="2">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B57" t="s" s="2">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C57" s="2"/>
       <c r="D57" t="s" s="2">
@@ -8209,32 +8222,28 @@
         <v>36</v>
       </c>
       <c r="I57" t="s" s="2">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="J57" t="s" s="2">
         <v>36</v>
       </c>
       <c r="K57" t="s" s="2">
+        <v>177</v>
+      </c>
+      <c r="L57" t="s" s="2">
+        <v>397</v>
+      </c>
+      <c r="M57" t="s" s="2">
         <v>398</v>
       </c>
-      <c r="L57" t="s" s="2">
+      <c r="N57" t="s" s="2">
         <v>399</v>
       </c>
-      <c r="M57" t="s" s="2">
-        <v>400</v>
-      </c>
-      <c r="N57" t="s" s="2">
-        <v>401</v>
-      </c>
-      <c r="O57" t="s" s="2">
-        <v>402</v>
-      </c>
+      <c r="O57" s="2"/>
       <c r="P57" t="s" s="2">
         <v>36</v>
       </c>
-      <c r="Q57" t="s" s="2">
-        <v>403</v>
-      </c>
+      <c r="Q57" s="2"/>
       <c r="R57" t="s" s="2">
         <v>36</v>
       </c>
@@ -8278,7 +8287,7 @@
         <v>36</v>
       </c>
       <c r="AF57" t="s" s="2">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="AG57" t="s" s="2">
         <v>34</v>
@@ -8293,10 +8302,10 @@
         <v>55</v>
       </c>
       <c r="AK57" t="s" s="2">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="AL57" t="s" s="2">
-        <v>405</v>
+        <v>36</v>
       </c>
       <c r="AM57" t="s" s="2">
         <v>36</v>
@@ -8307,10 +8316,10 @@
     </row>
     <row r="58">
       <c r="A58" t="s" s="2">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="B58" t="s" s="2">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="C58" s="2"/>
       <c r="D58" t="s" s="2">
@@ -8327,28 +8336,32 @@
         <v>36</v>
       </c>
       <c r="I58" t="s" s="2">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="J58" t="s" s="2">
         <v>36</v>
       </c>
       <c r="K58" t="s" s="2">
+        <v>402</v>
+      </c>
+      <c r="L58" t="s" s="2">
+        <v>403</v>
+      </c>
+      <c r="M58" t="s" s="2">
+        <v>404</v>
+      </c>
+      <c r="N58" t="s" s="2">
+        <v>405</v>
+      </c>
+      <c r="O58" t="s" s="2">
+        <v>406</v>
+      </c>
+      <c r="P58" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="Q58" t="s" s="2">
         <v>407</v>
       </c>
-      <c r="L58" t="s" s="2">
-        <v>408</v>
-      </c>
-      <c r="M58" t="s" s="2">
-        <v>409</v>
-      </c>
-      <c r="N58" s="2"/>
-      <c r="O58" t="s" s="2">
-        <v>410</v>
-      </c>
-      <c r="P58" t="s" s="2">
-        <v>36</v>
-      </c>
-      <c r="Q58" s="2"/>
       <c r="R58" t="s" s="2">
         <v>36</v>
       </c>
@@ -8392,7 +8405,7 @@
         <v>36</v>
       </c>
       <c r="AF58" t="s" s="2">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="AG58" t="s" s="2">
         <v>34</v>
@@ -8407,24 +8420,24 @@
         <v>55</v>
       </c>
       <c r="AK58" t="s" s="2">
-        <v>220</v>
+        <v>408</v>
       </c>
       <c r="AL58" t="s" s="2">
-        <v>221</v>
+        <v>409</v>
       </c>
       <c r="AM58" t="s" s="2">
         <v>36</v>
       </c>
       <c r="AN58" t="s" s="2">
-        <v>411</v>
+        <v>36</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s" s="2">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="B59" t="s" s="2">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="C59" s="2"/>
       <c r="D59" t="s" s="2">
@@ -8447,19 +8460,17 @@
         <v>36</v>
       </c>
       <c r="K59" t="s" s="2">
+        <v>411</v>
+      </c>
+      <c r="L59" t="s" s="2">
+        <v>412</v>
+      </c>
+      <c r="M59" t="s" s="2">
         <v>413</v>
       </c>
-      <c r="L59" t="s" s="2">
+      <c r="N59" s="2"/>
+      <c r="O59" t="s" s="2">
         <v>414</v>
-      </c>
-      <c r="M59" t="s" s="2">
-        <v>415</v>
-      </c>
-      <c r="N59" t="s" s="2">
-        <v>416</v>
-      </c>
-      <c r="O59" t="s" s="2">
-        <v>417</v>
       </c>
       <c r="P59" t="s" s="2">
         <v>36</v>
@@ -8508,7 +8519,7 @@
         <v>36</v>
       </c>
       <c r="AF59" t="s" s="2">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="AG59" t="s" s="2">
         <v>34</v>
@@ -8523,24 +8534,24 @@
         <v>55</v>
       </c>
       <c r="AK59" t="s" s="2">
-        <v>36</v>
+        <v>220</v>
       </c>
       <c r="AL59" t="s" s="2">
-        <v>418</v>
+        <v>221</v>
       </c>
       <c r="AM59" t="s" s="2">
         <v>36</v>
       </c>
       <c r="AN59" t="s" s="2">
-        <v>419</v>
+        <v>415</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s" s="2">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="B60" t="s" s="2">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="C60" s="2"/>
       <c r="D60" t="s" s="2">
@@ -8551,7 +8562,7 @@
         <v>34</v>
       </c>
       <c r="G60" t="s" s="2">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="H60" t="s" s="2">
         <v>36</v>
@@ -8563,19 +8574,19 @@
         <v>36</v>
       </c>
       <c r="K60" t="s" s="2">
+        <v>417</v>
+      </c>
+      <c r="L60" t="s" s="2">
+        <v>418</v>
+      </c>
+      <c r="M60" t="s" s="2">
+        <v>419</v>
+      </c>
+      <c r="N60" t="s" s="2">
+        <v>420</v>
+      </c>
+      <c r="O60" t="s" s="2">
         <v>421</v>
-      </c>
-      <c r="L60" t="s" s="2">
-        <v>422</v>
-      </c>
-      <c r="M60" t="s" s="2">
-        <v>423</v>
-      </c>
-      <c r="N60" t="s" s="2">
-        <v>424</v>
-      </c>
-      <c r="O60" t="s" s="2">
-        <v>417</v>
       </c>
       <c r="P60" t="s" s="2">
         <v>36</v>
@@ -8624,13 +8635,13 @@
         <v>36</v>
       </c>
       <c r="AF60" t="s" s="2">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="AG60" t="s" s="2">
         <v>34</v>
       </c>
       <c r="AH60" t="s" s="2">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="AI60" t="s" s="2">
         <v>36</v>
@@ -8639,24 +8650,24 @@
         <v>55</v>
       </c>
       <c r="AK60" t="s" s="2">
-        <v>425</v>
+        <v>36</v>
       </c>
       <c r="AL60" t="s" s="2">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="AM60" t="s" s="2">
         <v>36</v>
       </c>
       <c r="AN60" t="s" s="2">
-        <v>427</v>
+        <v>423</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s" s="2">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="B61" t="s" s="2">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="C61" s="2"/>
       <c r="D61" t="s" s="2">
@@ -8667,7 +8678,7 @@
         <v>34</v>
       </c>
       <c r="G61" t="s" s="2">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="H61" t="s" s="2">
         <v>36</v>
@@ -8679,16 +8690,20 @@
         <v>36</v>
       </c>
       <c r="K61" t="s" s="2">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="L61" t="s" s="2">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="M61" t="s" s="2">
-        <v>431</v>
-      </c>
-      <c r="N61" s="2"/>
-      <c r="O61" s="2"/>
+        <v>427</v>
+      </c>
+      <c r="N61" t="s" s="2">
+        <v>428</v>
+      </c>
+      <c r="O61" t="s" s="2">
+        <v>421</v>
+      </c>
       <c r="P61" t="s" s="2">
         <v>36</v>
       </c>
@@ -8712,13 +8727,13 @@
         <v>36</v>
       </c>
       <c r="X61" t="s" s="2">
-        <v>182</v>
+        <v>36</v>
       </c>
       <c r="Y61" t="s" s="2">
-        <v>432</v>
+        <v>36</v>
       </c>
       <c r="Z61" t="s" s="2">
-        <v>433</v>
+        <v>36</v>
       </c>
       <c r="AA61" t="s" s="2">
         <v>36</v>
@@ -8736,13 +8751,13 @@
         <v>36</v>
       </c>
       <c r="AF61" t="s" s="2">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="AG61" t="s" s="2">
         <v>34</v>
       </c>
       <c r="AH61" t="s" s="2">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="AI61" t="s" s="2">
         <v>36</v>
@@ -8751,28 +8766,28 @@
         <v>55</v>
       </c>
       <c r="AK61" t="s" s="2">
-        <v>36</v>
+        <v>429</v>
       </c>
       <c r="AL61" t="s" s="2">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="AM61" t="s" s="2">
         <v>36</v>
       </c>
       <c r="AN61" t="s" s="2">
-        <v>435</v>
+        <v>431</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s" s="2">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="B62" t="s" s="2">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="C62" s="2"/>
       <c r="D62" t="s" s="2">
-        <v>437</v>
+        <v>36</v>
       </c>
       <c r="E62" s="2"/>
       <c r="F62" t="s" s="2">
@@ -8791,18 +8806,16 @@
         <v>36</v>
       </c>
       <c r="K62" t="s" s="2">
-        <v>438</v>
+        <v>433</v>
       </c>
       <c r="L62" t="s" s="2">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="M62" t="s" s="2">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="N62" s="2"/>
-      <c r="O62" t="s" s="2">
-        <v>441</v>
-      </c>
+      <c r="O62" s="2"/>
       <c r="P62" t="s" s="2">
         <v>36</v>
       </c>
@@ -8826,13 +8839,13 @@
         <v>36</v>
       </c>
       <c r="X62" t="s" s="2">
-        <v>36</v>
+        <v>182</v>
       </c>
       <c r="Y62" t="s" s="2">
-        <v>36</v>
+        <v>436</v>
       </c>
       <c r="Z62" t="s" s="2">
-        <v>36</v>
+        <v>437</v>
       </c>
       <c r="AA62" t="s" s="2">
         <v>36</v>
@@ -8850,7 +8863,7 @@
         <v>36</v>
       </c>
       <c r="AF62" t="s" s="2">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="AG62" t="s" s="2">
         <v>34</v>
@@ -8868,25 +8881,25 @@
         <v>36</v>
       </c>
       <c r="AL62" t="s" s="2">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="AM62" t="s" s="2">
         <v>36</v>
       </c>
       <c r="AN62" t="s" s="2">
-        <v>443</v>
+        <v>439</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s" s="2">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="B63" t="s" s="2">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="C63" s="2"/>
       <c r="D63" t="s" s="2">
-        <v>36</v>
+        <v>441</v>
       </c>
       <c r="E63" s="2"/>
       <c r="F63" t="s" s="2">
@@ -8905,16 +8918,18 @@
         <v>36</v>
       </c>
       <c r="K63" t="s" s="2">
-        <v>438</v>
+        <v>442</v>
       </c>
       <c r="L63" t="s" s="2">
+        <v>443</v>
+      </c>
+      <c r="M63" t="s" s="2">
+        <v>444</v>
+      </c>
+      <c r="N63" s="2"/>
+      <c r="O63" t="s" s="2">
         <v>445</v>
       </c>
-      <c r="M63" t="s" s="2">
-        <v>446</v>
-      </c>
-      <c r="N63" s="2"/>
-      <c r="O63" s="2"/>
       <c r="P63" t="s" s="2">
         <v>36</v>
       </c>
@@ -8962,7 +8977,7 @@
         <v>36</v>
       </c>
       <c r="AF63" t="s" s="2">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="AG63" t="s" s="2">
         <v>34</v>
@@ -8980,21 +8995,21 @@
         <v>36</v>
       </c>
       <c r="AL63" t="s" s="2">
+        <v>446</v>
+      </c>
+      <c r="AM63" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="AN63" t="s" s="2">
         <v>447</v>
-      </c>
-      <c r="AM63" t="s" s="2">
-        <v>36</v>
-      </c>
-      <c r="AN63" t="s" s="2">
-        <v>448</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s" s="2">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B64" t="s" s="2">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C64" s="2"/>
       <c r="D64" t="s" s="2">
@@ -9017,13 +9032,13 @@
         <v>36</v>
       </c>
       <c r="K64" t="s" s="2">
-        <v>187</v>
+        <v>442</v>
       </c>
       <c r="L64" t="s" s="2">
+        <v>449</v>
+      </c>
+      <c r="M64" t="s" s="2">
         <v>450</v>
-      </c>
-      <c r="M64" t="s" s="2">
-        <v>451</v>
       </c>
       <c r="N64" s="2"/>
       <c r="O64" s="2"/>
@@ -9074,7 +9089,7 @@
         <v>36</v>
       </c>
       <c r="AF64" t="s" s="2">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="AG64" t="s" s="2">
         <v>34</v>
@@ -9092,13 +9107,13 @@
         <v>36</v>
       </c>
       <c r="AL64" t="s" s="2">
+        <v>451</v>
+      </c>
+      <c r="AM64" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="AN64" t="s" s="2">
         <v>452</v>
-      </c>
-      <c r="AM64" t="s" s="2">
-        <v>36</v>
-      </c>
-      <c r="AN64" t="s" s="2">
-        <v>324</v>
       </c>
     </row>
     <row r="65">
@@ -9117,7 +9132,7 @@
         <v>34</v>
       </c>
       <c r="G65" t="s" s="2">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="H65" t="s" s="2">
         <v>36</v>
@@ -9129,7 +9144,7 @@
         <v>36</v>
       </c>
       <c r="K65" t="s" s="2">
-        <v>318</v>
+        <v>187</v>
       </c>
       <c r="L65" t="s" s="2">
         <v>454</v>
@@ -9138,9 +9153,7 @@
         <v>455</v>
       </c>
       <c r="N65" s="2"/>
-      <c r="O65" t="s" s="2">
-        <v>456</v>
-      </c>
+      <c r="O65" s="2"/>
       <c r="P65" t="s" s="2">
         <v>36</v>
       </c>
@@ -9194,7 +9207,7 @@
         <v>34</v>
       </c>
       <c r="AH65" t="s" s="2">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="AI65" t="s" s="2">
         <v>36</v>
@@ -9203,16 +9216,130 @@
         <v>55</v>
       </c>
       <c r="AK65" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="AL65" t="s" s="2">
+        <v>456</v>
+      </c>
+      <c r="AM65" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="AN65" t="s" s="2">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="s" s="2">
         <v>457</v>
       </c>
-      <c r="AL65" t="s" s="2">
-        <v>323</v>
-      </c>
-      <c r="AM65" t="s" s="2">
-        <v>36</v>
-      </c>
-      <c r="AN65" t="s" s="2">
-        <v>324</v>
+      <c r="B66" t="s" s="2">
+        <v>457</v>
+      </c>
+      <c r="C66" s="2"/>
+      <c r="D66" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="E66" s="2"/>
+      <c r="F66" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="G66" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="H66" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="I66" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="J66" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="K66" t="s" s="2">
+        <v>322</v>
+      </c>
+      <c r="L66" t="s" s="2">
+        <v>458</v>
+      </c>
+      <c r="M66" t="s" s="2">
+        <v>459</v>
+      </c>
+      <c r="N66" s="2"/>
+      <c r="O66" t="s" s="2">
+        <v>460</v>
+      </c>
+      <c r="P66" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="Q66" s="2"/>
+      <c r="R66" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="S66" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="T66" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="U66" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="V66" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="W66" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="X66" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="Y66" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="Z66" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="AA66" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="AB66" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="AC66" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="AD66" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="AE66" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="AF66" t="s" s="2">
+        <v>457</v>
+      </c>
+      <c r="AG66" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="AH66" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="AI66" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="AJ66" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="AK66" t="s" s="2">
+        <v>461</v>
+      </c>
+      <c r="AL66" t="s" s="2">
+        <v>327</v>
+      </c>
+      <c r="AM66" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="AN66" t="s" s="2">
+        <v>328</v>
       </c>
     </row>
   </sheetData>

</xml_diff>